<commit_message>
Add list courses, statistical sourses of registeration
</commit_message>
<xml_diff>
--- a/StudentManagement/excels/student.xlsx
+++ b/StudentManagement/excels/student.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaProject\StudentManagement\StudentManagement\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\StudentManagement\StudentManagement\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB138D7C-4F9F-457C-BC5D-59B2F46A99A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C221078-D2D1-4013-A143-1DB12D2FF12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -252,27 +252,9 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Sdth</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Ngày sinh</t>
-  </si>
-  <si>
-    <t>Quê</t>
-  </si>
-  <si>
-    <t>Giới tính</t>
-  </si>
-  <si>
-    <t>CMND</t>
-  </si>
-  <si>
-    <t>Chỗ ở hiện tại</t>
-  </si>
-  <si>
     <t>RegisterType</t>
   </si>
   <si>
@@ -292,6 +274,24 @@
   </si>
   <si>
     <t>K05</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Day Of Birth</t>
+  </si>
+  <si>
+    <t>HomeTown</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>IdNumber</t>
+  </si>
+  <si>
+    <t>CurrentAddress</t>
   </si>
 </sst>
 </file>
@@ -578,22 +578,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99485173-C7E8-4E33-8869-BA7684B808A7}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="4" width="32.75" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="24.796875" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" customWidth="1"/>
+    <col min="4" max="4" width="32.69921875" customWidth="1"/>
+    <col min="5" max="5" width="15.3984375" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="30.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.125" customWidth="1"/>
-    <col min="11" max="11" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.59765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.09765625" customWidth="1"/>
+    <col min="11" max="11" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
@@ -604,31 +604,31 @@
         <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1">
@@ -663,7 +663,7 @@
         <v>4</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -733,7 +733,7 @@
         <v>4</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -768,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -803,7 +803,7 @@
         <v>4</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -838,7 +838,7 @@
         <v>23</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -873,7 +873,7 @@
         <v>23</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -908,7 +908,7 @@
         <v>23</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -943,7 +943,7 @@
         <v>23</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -978,7 +978,7 @@
         <v>34</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1013,7 +1013,7 @@
         <v>34</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1048,7 +1048,7 @@
         <v>34</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1083,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1118,7 +1118,7 @@
         <v>34</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1153,7 +1153,7 @@
         <v>34</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1188,7 +1188,7 @@
         <v>23</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1223,7 +1223,7 @@
         <v>4</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1258,7 +1258,7 @@
         <v>34</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1293,7 +1293,7 @@
         <v>23</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1328,7 +1328,7 @@
         <v>34</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1363,7 +1363,7 @@
         <v>23</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1398,7 +1398,7 @@
         <v>34</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1433,7 +1433,7 @@
         <v>23</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1468,7 +1468,7 @@
         <v>34</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1503,7 +1503,7 @@
         <v>23</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>